<commit_message>
updated source plate DA
</commit_message>
<xml_diff>
--- a/source_plates/211129_ECHO_source_plate.xlsx
+++ b/source_plates/211129_ECHO_source_plate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\WHISPR\source_plates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F3FF5C-6922-44D4-A0FC-139F92110521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B6A2EE-F9C1-4071-835B-3067E67A5575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{546D7F41-76BF-4117-BD41-03A67E651BAB}"/>
+    <workbookView xWindow="23430" yWindow="1785" windowWidth="12870" windowHeight="14085" xr2:uid="{546D7F41-76BF-4117-BD41-03A67E651BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="ECHO_source_plate" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>C4, C5, A2,A3,A4,A5,A6,A7,A8,A9,A10,A11,A12</t>
   </si>
   <si>
-    <t>50,50,50,65,65,65,65,65,65,65,65,65,65,65</t>
-  </si>
-  <si>
     <t>pBT009.J1.117.J306</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>D5</t>
+  </si>
+  <si>
+    <t>19.475,50,50,65,65,65,65,65,65,65,65,65,65,65</t>
   </si>
 </sst>
 </file>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D29ACC-8067-425A-9239-04930501B2E7}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="142" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +707,7 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -732,13 +732,13 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
       </c>
       <c r="D3">
         <v>511</v>
@@ -769,13 +769,13 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
       </c>
       <c r="D4">
         <v>223</v>
@@ -806,13 +806,13 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
       </c>
       <c r="D5">
         <v>115.5</v>
@@ -843,13 +843,13 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
       </c>
       <c r="D6">
         <v>157</v>
@@ -880,13 +880,13 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
       </c>
       <c r="D7">
         <v>116.6</v>
@@ -917,13 +917,13 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
       </c>
       <c r="D8">
         <v>135.69999999999999</v>
@@ -954,13 +954,13 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
       </c>
       <c r="D9">
         <v>190.3</v>
@@ -991,13 +991,13 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
       </c>
       <c r="D10">
         <v>189.3</v>
@@ -1008,13 +1008,13 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
         <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
       </c>
       <c r="D11">
         <v>40</v>
@@ -1051,13 +1051,13 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>188</v>
       </c>
       <c r="E12">
-        <v>55</v>
+        <v>51.274999999999999</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1085,10 +1085,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
       </c>
       <c r="D13">
         <v>1.88</v>
@@ -1105,13 +1105,13 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14">
         <v>356</v>
       </c>
       <c r="E14">
-        <v>46</v>
+        <v>43.9</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1136,13 +1136,13 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
         <v>47</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
       </c>
       <c r="D15">
         <v>237.9</v>
@@ -1173,13 +1173,13 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
       </c>
       <c r="D16">
         <v>2.379</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
       </c>
       <c r="D17">
         <v>0.2379</v>
@@ -1239,7 +1239,7 @@
         <v>222</v>
       </c>
       <c r="E18">
-        <v>50</v>
+        <v>49.95</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,10 +1278,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -1295,10 +1295,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1312,10 +1312,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -1346,10 +1346,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
@@ -1403,7 +1403,7 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28">
         <v>120.7</v>
@@ -1420,7 +1420,7 @@
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29">
         <v>117</v>
@@ -1434,87 +1434,87 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>66</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
       </c>
       <c r="D31">
         <v>226.9</v>
       </c>
       <c r="E31">
-        <v>60</v>
+        <v>49.3</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32">
         <v>2.2690000000000001</v>
       </c>
       <c r="E32">
-        <v>60</v>
+        <v>53.725000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33">
         <v>149</v>
       </c>
       <c r="E33">
-        <v>60</v>
+        <v>50.274999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34">
         <v>151.5</v>
       </c>
       <c r="E34">
-        <v>60</v>
+        <v>50.45</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35">
         <v>185</v>
       </c>
       <c r="E35">
-        <v>60</v>
+        <v>51.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>